<commit_message>
updated datatable for logo e2e
</commit_message>
<xml_diff>
--- a/automationdemo.maven/testdata/manageLogo.xlsx
+++ b/automationdemo.maven/testdata/manageLogo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C839E73-54EE-4700-80C3-22286DD985AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A007FBAD-BC44-4E82-8E98-EF95059D7ACF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22770" yWindow="-16515" windowWidth="14505" windowHeight="10980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindetails" sheetId="1" r:id="rId1"/>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DA3203-5EC9-4931-89A5-BD9BB2B4C6EF}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -565,9 +565,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>